<commit_message>
started the analysis on breakdowning down the incident by type depending on keywords in the description
</commit_message>
<xml_diff>
--- a/data_2.xlsx
+++ b/data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/theme_park_accidents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6053E1-3189-7244-8D44-991C624C8014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E40B681-DDC7-DC4C-8611-F76B8B9F0AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="20120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,13 +21,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="701">
   <si>
     <t>Company</t>
   </si>
@@ -2616,16 +2616,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3065,7 +3068,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -14603,7 +14606,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE3CD5F5-40E6-8148-B587-8AD4EC3E6391}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE3CD5F5-40E6-8148-B587-8AD4EC3E6391}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A29:B42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0">
@@ -14772,7 +14775,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{727F7744-D220-DB4C-A3FC-79013D27B66F}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{727F7744-D220-DB4C-A3FC-79013D27B66F}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0">
@@ -14964,7 +14967,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6C1F810E-E08E-D344-BC28-D7CDD42BBDC3}" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6C1F810E-E08E-D344-BC28-D7CDD42BBDC3}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0">
@@ -15081,7 +15084,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C6C314CD-B818-7F42-B1CF-2E4C4DD4449B}" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C6C314CD-B818-7F42-B1CF-2E4C4DD4449B}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0">
@@ -15164,10 +15167,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A160A795-00B7-204E-8DB9-C45015474760}" name="PivotTable5" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A160A795-00B7-204E-8DB9-C45015474760}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
-    <pivotField dataField="1" showAll="0">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -15193,7 +15196,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
+    <pivotField showAll="0">
       <items count="113">
         <item x="0"/>
         <item x="1"/>
@@ -15309,17 +15312,8 @@
         <item x="111"/>
         <item t="default"/>
       </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
     </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+    <pivotField multipleItemSelectionAllowed="1" showAll="0">
       <items count="10">
         <item h="1" x="2"/>
         <item h="1" x="5"/>
@@ -15335,7 +15329,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="516">
         <item x="477"/>
         <item x="159"/>
@@ -15894,57 +15888,82 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="25">
     <i>
+      <x/>
+    </i>
+    <i r="1">
       <x v="33"/>
     </i>
-    <i>
-      <x v="97"/>
+    <i r="1">
+      <x v="39"/>
+    </i>
+    <i r="1">
+      <x v="48"/>
+    </i>
+    <i r="1">
+      <x v="55"/>
+    </i>
+    <i r="1">
+      <x v="93"/>
+    </i>
+    <i r="1">
+      <x v="148"/>
+    </i>
+    <i r="1">
+      <x v="169"/>
+    </i>
+    <i r="1">
+      <x v="174"/>
+    </i>
+    <i r="1">
+      <x v="204"/>
+    </i>
+    <i r="1">
+      <x v="258"/>
+    </i>
+    <i r="1">
+      <x v="281"/>
+    </i>
+    <i r="1">
+      <x v="282"/>
+    </i>
+    <i r="1">
+      <x v="296"/>
+    </i>
+    <i r="1">
+      <x v="306"/>
+    </i>
+    <i r="1">
+      <x v="361"/>
+    </i>
+    <i r="1">
+      <x v="370"/>
+    </i>
+    <i r="1">
+      <x v="378"/>
+    </i>
+    <i r="1">
+      <x v="397"/>
+    </i>
+    <i r="1">
+      <x v="400"/>
+    </i>
+    <i r="1">
+      <x v="422"/>
+    </i>
+    <i r="1">
+      <x v="442"/>
     </i>
     <i>
-      <x v="18"/>
+      <x v="1"/>
     </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="94"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="65"/>
-    </i>
-    <i>
-      <x v="96"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="84"/>
-    </i>
-    <i>
-      <x v="38"/>
+    <i r="1">
+      <x v="464"/>
     </i>
     <i t="grand">
       <x/>
@@ -15953,13 +15972,21 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Company" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="6" type="captionContains" evalOrder="-1" id="8" stringValue1="passed away">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter val="*passed away*"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -16297,7 +16324,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>660</v>
       </c>
       <c r="B3" t="s">
@@ -16305,191 +16332,191 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>684</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>686</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>692</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>682</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>660</v>
       </c>
       <c r="B29" t="s">
@@ -16497,106 +16524,106 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42">
         <v>682</v>
       </c>
     </row>
@@ -16621,7 +16648,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>660</v>
       </c>
       <c r="B3" t="s">
@@ -16629,82 +16656,82 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>682</v>
       </c>
     </row>
@@ -16729,7 +16756,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>660</v>
       </c>
       <c r="B3" t="s">
@@ -16737,50 +16764,50 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>682</v>
       </c>
     </row>
@@ -16792,28 +16819,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA98957-F91A-1B45-866C-C78F82158C85}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A3:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="134.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>660</v>
       </c>
       <c r="B3" t="s">
@@ -16821,139 +16840,203 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B4" s="2">
-        <v>43</v>
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>585</v>
-      </c>
-      <c r="B5" s="2">
-        <v>11</v>
+      <c r="A5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="2">
-        <v>11</v>
+      <c r="A6" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
+      <c r="A7" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="2">
-        <v>4</v>
+      <c r="A8" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
+      <c r="A9" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3</v>
+      <c r="A10" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="2">
-        <v>3</v>
+      <c r="A11" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2</v>
+      <c r="A12" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
+      <c r="A13" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2</v>
+      <c r="A14" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>584</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B16" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="B18" s="2">
+      <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="A19" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="B19" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="B20" s="2">
-        <v>95</v>
+      <c r="B28" s="5">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>